<commit_message>
Fixed error in peak forces
</commit_message>
<xml_diff>
--- a/example_excel_test/example_template.xlsx
+++ b/example_excel_test/example_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Projects\MECH2100-A2\example_excel_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2946F8-3E3A-4078-9A5E-6EBC13B0A693}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33A2423-0160-4AEE-B197-8095522D3149}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13452" yWindow="4944" windowWidth="17136" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35505" yWindow="2265" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1338,13 +1338,13 @@
         <v>46</v>
       </c>
       <c r="F25" s="11">
-        <v>88895.956414094137</v>
+        <v>88895.956414094151</v>
       </c>
       <c r="G25" s="11">
-        <v>44447.978207047068</v>
+        <v>44447.978207047076</v>
       </c>
       <c r="H25" s="11">
-        <v>26668.786924228243</v>
+        <v>26668.78692422825</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="2" t="s">
@@ -1744,13 +1744,13 @@
         <v>91</v>
       </c>
       <c r="F59" s="15">
-        <v>-222239.89103523534</v>
+        <v>-222239.89103523537</v>
       </c>
       <c r="G59" s="15">
-        <v>-111119.94551761767</v>
+        <v>-111119.94551761769</v>
       </c>
       <c r="H59" s="15">
-        <v>-66671.967310570602</v>
+        <v>-66671.967310570632</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>92</v>
@@ -1770,13 +1770,13 @@
         <v>91</v>
       </c>
       <c r="F60" s="15">
-        <v>-133343.9346211412</v>
+        <v>-133343.93462114123</v>
       </c>
       <c r="G60" s="15">
-        <v>-66671.967310570602</v>
+        <v>-66671.967310570617</v>
       </c>
       <c r="H60" s="15">
-        <v>-40003.180386342356</v>
+        <v>-40003.180386342385</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>92</v>
@@ -1796,13 +1796,13 @@
         <v>91</v>
       </c>
       <c r="F61" s="15">
-        <v>-44447.978207047068</v>
+        <v>-44447.978207047083</v>
       </c>
       <c r="G61" s="15">
-        <v>-22223.989103523534</v>
+        <v>-22223.989103523541</v>
       </c>
       <c r="H61" s="15">
-        <v>-13334.393462114112</v>
+        <v>-13334.393462114138</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>92</v>
@@ -1822,13 +1822,13 @@
         <v>91</v>
       </c>
       <c r="F62" s="15">
-        <v>177791.91282818827</v>
+        <v>177791.9128281883</v>
       </c>
       <c r="G62" s="15">
-        <v>88895.956414094137</v>
+        <v>88895.956414094151</v>
       </c>
       <c r="H62" s="15">
-        <v>53337.573848456479</v>
+        <v>53337.573848456508</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>92</v>
@@ -1848,13 +1848,13 @@
         <v>91</v>
       </c>
       <c r="F63" s="15">
-        <v>88895.956414094137</v>
+        <v>88895.956414094151</v>
       </c>
       <c r="G63" s="15">
-        <v>44447.978207047068</v>
+        <v>44447.978207047076</v>
       </c>
       <c r="H63" s="15">
-        <v>26668.786924228236</v>
+        <v>26668.786924228261</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>92</v>
@@ -1900,13 +1900,13 @@
         <v>91</v>
       </c>
       <c r="F65" s="15">
-        <v>-44447.978207047068</v>
+        <v>-44447.978207047076</v>
       </c>
       <c r="G65" s="15">
-        <v>-22223.989103523534</v>
+        <v>-22223.989103523538</v>
       </c>
       <c r="H65" s="15">
-        <v>-13334.393462114122</v>
+        <v>-13334.393462114125</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>92</v>
@@ -1926,13 +1926,13 @@
         <v>91</v>
       </c>
       <c r="F66" s="15">
-        <v>62858.933600469725</v>
+        <v>62858.933600469732</v>
       </c>
       <c r="G66" s="15">
-        <v>31429.466800234863</v>
+        <v>31429.466800234866</v>
       </c>
       <c r="H66" s="15">
-        <v>18857.680080140919</v>
+        <v>18857.680080140923</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>92</v>
@@ -1952,13 +1952,13 @@
         <v>91</v>
       </c>
       <c r="F67" s="15">
-        <v>-62858.933600469725</v>
+        <v>-62858.933600469732</v>
       </c>
       <c r="G67" s="15">
-        <v>-31429.466800234863</v>
+        <v>-31429.466800234866</v>
       </c>
       <c r="H67" s="15">
-        <v>-18857.680080140919</v>
+        <v>-18857.680080140923</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>92</v>
@@ -1978,13 +1978,13 @@
         <v>91</v>
       </c>
       <c r="F68" s="15">
-        <v>62858.933600469725</v>
+        <v>62858.933600469732</v>
       </c>
       <c r="G68" s="15">
-        <v>31429.466800234863</v>
+        <v>31429.466800234866</v>
       </c>
       <c r="H68" s="15">
-        <v>18857.680080140919</v>
+        <v>18857.680080140923</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>92</v>
@@ -2004,13 +2004,13 @@
         <v>91</v>
       </c>
       <c r="F69" s="15">
-        <v>-62858.933600469725</v>
+        <v>-62858.933600469732</v>
       </c>
       <c r="G69" s="15">
-        <v>-31429.466800234863</v>
+        <v>-31429.466800234866</v>
       </c>
       <c r="H69" s="15">
-        <v>-18857.680080140919</v>
+        <v>-18857.680080140923</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>92</v>
@@ -2030,13 +2030,13 @@
         <v>91</v>
       </c>
       <c r="F70" s="15">
-        <v>62858.933600469725</v>
+        <v>62858.933600469732</v>
       </c>
       <c r="G70" s="15">
-        <v>31429.466800234863</v>
+        <v>31429.466800234866</v>
       </c>
       <c r="H70" s="15">
-        <v>18857.680080140919</v>
+        <v>18857.680080140923</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>92</v>
@@ -2056,13 +2056,13 @@
         <v>91</v>
       </c>
       <c r="F71" s="15">
-        <v>-44447.978207047068</v>
+        <v>-44447.978207047076</v>
       </c>
       <c r="G71" s="15">
-        <v>-22223.989103523534</v>
+        <v>-22223.989103523538</v>
       </c>
       <c r="H71" s="15">
-        <v>-13334.393462114122</v>
+        <v>-13334.393462114125</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>92</v>
@@ -2141,13 +2141,13 @@
         <v>106</v>
       </c>
       <c r="F78" s="15">
-        <v>-222239.89103523534</v>
+        <v>-222239.89103523537</v>
       </c>
       <c r="G78" s="15">
-        <v>-111119.94551761767</v>
+        <v>-111119.94551761769</v>
       </c>
       <c r="H78" s="15">
-        <v>-66671.967310570602</v>
+        <v>-66671.967310570632</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
@@ -2164,13 +2164,13 @@
         <v>108</v>
       </c>
       <c r="F79" s="15">
-        <v>44447.978207047068</v>
+        <v>44447.978207047076</v>
       </c>
       <c r="G79" s="15">
-        <v>22223.989103523534</v>
+        <v>22223.989103523538</v>
       </c>
       <c r="H79" s="15">
-        <v>13334.393462114122</v>
+        <v>13334.393462114125</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>84</v>
@@ -2190,13 +2190,13 @@
         <v>110</v>
       </c>
       <c r="F80" s="15">
-        <v>222239.89103523534</v>
+        <v>222239.89103523537</v>
       </c>
       <c r="G80" s="15">
-        <v>111119.94551761767</v>
+        <v>111119.94551761769</v>
       </c>
       <c r="H80" s="15">
-        <v>66671.967310570602</v>
+        <v>66671.967310570632</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
@@ -2298,13 +2298,13 @@
         <v>114</v>
       </c>
       <c r="F96" s="14">
-        <v>35.348484407707041</v>
+        <v>35.348484407707048</v>
       </c>
       <c r="G96" s="14">
-        <v>17.67424220385352</v>
+        <v>17.674242203853524</v>
       </c>
       <c r="H96" s="14">
-        <v>10.604545322312113</v>
+        <v>10.604545322312122</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
@@ -2321,13 +2321,13 @@
         <v>114</v>
       </c>
       <c r="F97" s="14">
-        <v>-62.099999999999987</v>
+        <v>-62.099999999999994</v>
       </c>
       <c r="G97" s="14">
-        <v>-31.049999999999994</v>
+        <v>-31.049999999999997</v>
       </c>
       <c r="H97" s="14">
-        <v>-18.629999999999995</v>
+        <v>-18.63</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
@@ -2367,13 +2367,13 @@
         <v>114</v>
       </c>
       <c r="F99" s="14">
-        <v>62.099999999999987</v>
+        <v>62.099999999999994</v>
       </c>
       <c r="G99" s="14">
-        <v>31.049999999999994</v>
+        <v>31.049999999999997</v>
       </c>
       <c r="H99" s="14">
-        <v>18.629999999999995</v>
+        <v>18.63</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
@@ -2516,13 +2516,13 @@
         <v>119</v>
       </c>
       <c r="F123" s="14">
-        <v>53.022726611560572</v>
+        <v>53.022726611560579</v>
       </c>
       <c r="G123" s="14">
-        <v>26.511363305780286</v>
+        <v>26.511363305780289</v>
       </c>
       <c r="H123" s="14">
-        <v>15.906817983468169</v>
+        <v>15.906817983468182</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
@@ -2545,7 +2545,7 @@
         <v>-37.259999999999991</v>
       </c>
       <c r="H124" s="14">
-        <v>-22.355999999999995</v>
+        <v>-22.356000000000002</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
@@ -2591,7 +2591,7 @@
         <v>37.259999999999991</v>
       </c>
       <c r="H126" s="14">
-        <v>22.355999999999995</v>
+        <v>22.356000000000002</v>
       </c>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>